<commit_message>
Edit Demo1 Android Results
</commit_message>
<xml_diff>
--- a/4.- Plan de Pruebas/Demo 1 Resultados.xlsx
+++ b/4.- Plan de Pruebas/Demo 1 Resultados.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
   <si>
     <t>Sugerencias (WEB)</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Muchas pestañas iguales, ninguna destacada, o separada a la derecha (por ej contacto y encuesta a la dcha).</t>
   </si>
   <si>
-    <t>Varios contenidos dependientes de la misma pestaña y mover contacto a la derecha.</t>
-  </si>
-  <si>
     <t>El Acerca debería también estar fuera de "inicio".</t>
   </si>
   <si>
@@ -188,13 +185,22 @@
   </si>
   <si>
     <t>Esto ya estaba contemplado...</t>
+  </si>
+  <si>
+    <t>Varios contenidos dependientes de la misma pestaña y mover encuesta a la derecha.</t>
+  </si>
+  <si>
+    <t>Vamos a utilizarla para el perfil, settings y logout</t>
+  </si>
+  <si>
+    <t>Esto es código de google y si da tiempo intentaremos mejorarlo.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -209,6 +215,12 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -298,7 +310,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -340,6 +352,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -638,7 +653,7 @@
   <dimension ref="A1:U103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -687,7 +702,9 @@
       <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A3" s="7" t="s">
@@ -696,7 +713,9 @@
       <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="5"/>
+      <c r="C3" s="8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="4" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="2" t="s">
@@ -707,7 +726,7 @@
       </c>
       <c r="C4" s="5"/>
       <c r="D4" s="2" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -729,73 +748,81 @@
     </row>
     <row r="5" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A5" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="7" t="s">
         <v>9</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="7" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="5"/>
+      <c r="C6" s="8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A7" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="7" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="7" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A8" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="5"/>
-      <c r="D8" s="7" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="9" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" s="9" t="s">
-        <v>17</v>
       </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A10" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="10" t="s">
         <v>18</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>19</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>5</v>
@@ -804,31 +831,31 @@
     </row>
     <row r="12" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A13" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="5"/>
       <c r="D13" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A14" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>5</v>
@@ -837,7 +864,7 @@
     </row>
     <row r="15" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A15" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>5</v>
@@ -848,14 +875,14 @@
     </row>
     <row r="16" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A16" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="12.75" customHeight="1">
@@ -1217,7 +1244,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -1225,7 +1252,7 @@
     <col min="1" max="1" width="96" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="58.140625" customWidth="1"/>
+    <col min="4" max="4" width="58.140625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1">
@@ -1244,91 +1271,149 @@
     </row>
     <row r="2" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A5" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A7" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A8" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A9" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A10" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A11" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A12" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A13" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A14" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A15" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A16" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="7" customFormat="1" ht="30" customHeight="1">
+      <c r="A17" s="7" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" s="7" customFormat="1" ht="30" customHeight="1">
-      <c r="A17" s="7" t="s">
+      <c r="B17" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="7" customFormat="1" ht="38.25">
+      <c r="A18" s="7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" s="7" customFormat="1" ht="38.25">
-      <c r="A18" s="7" t="s">
-        <v>46</v>
+      <c r="B18" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1348,7 +1433,7 @@
     <col min="4" max="4" width="52" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="30">
+    <row r="1" spans="1:21" ht="15">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1381,7 +1466,7 @@
     </row>
     <row r="2" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>5</v>
@@ -1702,7 +1787,7 @@
     <col min="4" max="4" width="51.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="30">
+    <row r="1" spans="1:21" ht="15">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -1735,56 +1820,56 @@
     </row>
     <row r="2" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A2" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A3" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A4" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A5" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="13" t="s">
         <v>52</v>
-      </c>
-      <c r="B5" s="13" t="s">
-        <v>53</v>
       </c>
       <c r="C5" s="5"/>
       <c r="D5" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A6" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C6" s="5"/>
       <c r="D6" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="12.75" customHeight="1">

</xml_diff>

<commit_message>
Edit Demo1 Web Results
</commit_message>
<xml_diff>
--- a/4.- Plan de Pruebas/Demo 1 Resultados.xlsx
+++ b/4.- Plan de Pruebas/Demo 1 Resultados.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="59">
   <si>
     <t>Sugerencias (WEB)</t>
   </si>
@@ -653,7 +653,7 @@
   <dimension ref="A1:U103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -827,7 +827,9 @@
       <c r="B11" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="5"/>
+      <c r="C11" s="8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1">
       <c r="A12" s="7" t="s">
@@ -848,7 +850,9 @@
       <c r="B13" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="5"/>
+      <c r="C13" s="8" t="s">
+        <v>5</v>
+      </c>
       <c r="D13" s="7" t="s">
         <v>24</v>
       </c>
@@ -1243,7 +1247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Edit Demo1 Form Results
</commit_message>
<xml_diff>
--- a/4.- Plan de Pruebas/Demo 1 Resultados.xlsx
+++ b/4.- Plan de Pruebas/Demo 1 Resultados.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365"/>
+    <workbookView xWindow="360" yWindow="525" windowWidth="19815" windowHeight="7365" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="WEB" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="59">
   <si>
     <t>Sugerencias (WEB)</t>
   </si>
@@ -652,7 +652,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -1430,7 +1430,7 @@
   <dimension ref="A1:U100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="17.140625" defaultRowHeight="12.75" customHeight="1"/>
@@ -1479,6 +1479,9 @@
       <c r="B2" s="8" t="s">
         <v>5</v>
       </c>
+      <c r="C2" s="8" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="3" spans="1:21" ht="12.75" customHeight="1">
       <c r="B3" s="4"/>
@@ -1783,7 +1786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:U100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>